<commit_message>
Cloud deployment Compose file created
</commit_message>
<xml_diff>
--- a/Docs/Scrum planning en rapport template.xlsx
+++ b/Docs/Scrum planning en rapport template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rstep\OneDrive\Bureaublad\AP\J2\S2\AI-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecr\Documents\AP\2eJ-semester2\AI Project\AI-Project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AEF443-A4AB-4AF4-9967-D7A8D39A2AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B55863-AE16-4108-8C1F-627C45D40019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{E07F6153-1B8C-43A7-97BD-457FD435295E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{E07F6153-1B8C-43A7-97BD-457FD435295E}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="3" r:id="rId1"/>
@@ -1276,10 +1276,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1289,16 +1293,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="111">
     <dxf>
@@ -1630,10 +1630,38 @@
       </fill>
     </dxf>
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1644,38 +1672,10 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -1707,14 +1707,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AA82689C-D0AA-4F4B-919B-87E3028818E8}" name="Table4" displayName="Table4" ref="B14:D17" totalsRowShown="0" headerRowDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{AA82689C-D0AA-4F4B-919B-87E3028818E8}" name="Table4" displayName="Table4" ref="B14:D17" totalsRowShown="0" headerRowDxfId="110">
   <autoFilter ref="B14:D17" xr:uid="{AA82689C-D0AA-4F4B-919B-87E3028818E8}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5275A149-D9C7-4765-8593-A42F0BE5A234}" name="Status"/>
-    <tableColumn id="2" xr3:uid="{5D1A658E-6171-4853-98CD-6AB729C001BE}" name="Totaal aantal" dataDxfId="97">
+    <tableColumn id="2" xr3:uid="{5D1A658E-6171-4853-98CD-6AB729C001BE}" name="Totaal aantal" dataDxfId="109">
       <calculatedColumnFormula>COUNTIF(Backlog!$I$4:$I$52, B15)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8E35AA80-EB15-4700-9B95-52F62AF6B801}" name="Aantal SP" dataDxfId="96">
+    <tableColumn id="3" xr3:uid="{8E35AA80-EB15-4700-9B95-52F62AF6B801}" name="Aantal SP" dataDxfId="108">
       <calculatedColumnFormula>SUMIF(Backlog!$I$4:$I$52, B15, Backlog!$G$4:$G$52)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1742,24 +1742,24 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C31D63E-5C3E-42E3-BE92-09D26924F40D}" name="Table1" displayName="Table1" ref="A3:J36" totalsRowShown="0" headerRowDxfId="110" dataDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C31D63E-5C3E-42E3-BE92-09D26924F40D}" name="Table1" displayName="Table1" ref="A3:J36" totalsRowShown="0" headerRowDxfId="107" dataDxfId="106">
   <autoFilter ref="A3:J36" xr:uid="{0C31D63E-5C3E-42E3-BE92-09D26924F40D}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:J36">
     <sortCondition ref="A3:A36"/>
   </sortState>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{86C438A9-95F7-480B-8605-663A6D33F9E8}" name="GH Issue ID" dataDxfId="108"/>
-    <tableColumn id="2" xr3:uid="{A67F3775-FD76-4B45-9318-AEB1E2DDB617}" name="Naam" dataDxfId="107"/>
-    <tableColumn id="10" xr3:uid="{D71A8556-082B-4B32-B6BE-5BE60F40C14A}" name="Epic ID" dataDxfId="106"/>
-    <tableColumn id="3" xr3:uid="{C10F2FCC-7C0D-4C38-B585-FDBE69D8CB6A}" name="Omschrijving" dataDxfId="105"/>
-    <tableColumn id="4" xr3:uid="{B10BE454-0779-4408-827E-18CAFA3FA6F4}" name="Prioriteit" dataDxfId="104"/>
-    <tableColumn id="5" xr3:uid="{9DD6B241-13CA-4C6A-B38D-F66ABDFB4D1F}" name="Afhankelijkheden" dataDxfId="103">
+    <tableColumn id="1" xr3:uid="{86C438A9-95F7-480B-8605-663A6D33F9E8}" name="GH Issue ID" dataDxfId="105"/>
+    <tableColumn id="2" xr3:uid="{A67F3775-FD76-4B45-9318-AEB1E2DDB617}" name="Naam" dataDxfId="104"/>
+    <tableColumn id="10" xr3:uid="{D71A8556-082B-4B32-B6BE-5BE60F40C14A}" name="Epic ID" dataDxfId="103"/>
+    <tableColumn id="3" xr3:uid="{C10F2FCC-7C0D-4C38-B585-FDBE69D8CB6A}" name="Omschrijving" dataDxfId="102"/>
+    <tableColumn id="4" xr3:uid="{B10BE454-0779-4408-827E-18CAFA3FA6F4}" name="Prioriteit" dataDxfId="101"/>
+    <tableColumn id="5" xr3:uid="{9DD6B241-13CA-4C6A-B38D-F66ABDFB4D1F}" name="Afhankelijkheden" dataDxfId="100">
       <calculatedColumnFormula>A3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3917555F-8AC1-4D61-A1D1-AD989DECCDD8}" name="Story points" dataDxfId="102"/>
-    <tableColumn id="7" xr3:uid="{59A344ED-FCCF-4D1D-863D-3BC0B67970BA}" name="Sprint" dataDxfId="101"/>
-    <tableColumn id="8" xr3:uid="{7FB5F6F2-7561-43E7-940F-616623FD98C9}" name="Status" dataDxfId="100"/>
-    <tableColumn id="9" xr3:uid="{FC693D5F-36C5-47E3-8471-4017AADBBDA4}" name="Opmerkingen" dataDxfId="99"/>
+    <tableColumn id="6" xr3:uid="{3917555F-8AC1-4D61-A1D1-AD989DECCDD8}" name="Story points" dataDxfId="99"/>
+    <tableColumn id="7" xr3:uid="{59A344ED-FCCF-4D1D-863D-3BC0B67970BA}" name="Sprint" dataDxfId="98"/>
+    <tableColumn id="8" xr3:uid="{7FB5F6F2-7561-43E7-940F-616623FD98C9}" name="Status" dataDxfId="97"/>
+    <tableColumn id="9" xr3:uid="{FC693D5F-36C5-47E3-8471-4017AADBBDA4}" name="Opmerkingen" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1899,9 +1899,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Thema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1939,7 +1939,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2045,7 +2045,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2187,7 +2187,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="D8">
         <f>'Sprint 0'!F31+'Sprint 1'!F31+'Sprint 2'!F31+'Sprint 3'!F31+'Sprint 4'!F31+'Sprint 5'!F31+'Sprint 6'!F31+'Sprint 7'!F31</f>
-        <v>10</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -2279,7 +2279,7 @@
       </c>
       <c r="D9">
         <f>'Sprint 0'!G31+'Sprint 1'!G31+'Sprint 2'!G31+'Sprint 3'!G31+'Sprint 4'!G31+'Sprint 5'!G31+'Sprint 6'!G31+'Sprint 7'!G31</f>
-        <v>10</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="D10">
         <f>'Sprint 0'!H31+'Sprint 1'!H31+'Sprint 2'!H31+'Sprint 3'!H31+'Sprint 4'!H31+'Sprint 5'!H31+'Sprint 6'!H31+'Sprint 7'!H31</f>
-        <v>10.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -2769,144 +2769,150 @@
       <c r="A36" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="39"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="39"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="39"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="39"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -2916,12 +2922,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3316,144 +3316,150 @@
       <c r="A36" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="39"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="39"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="39"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="39"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -3463,12 +3469,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3481,7 +3481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77B3F3E5-4B5F-40F9-A800-013CC5F2EE00}">
   <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
@@ -3514,13 +3514,13 @@
       <c r="O1" s="14"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
       <c r="H2" s="14"/>
@@ -3533,11 +3533,11 @@
       <c r="O2" s="14"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="45"/>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
@@ -3550,11 +3550,11 @@
       <c r="O3" s="14"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -3567,11 +3567,11 @@
       <c r="O4" s="14"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="36"/>
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
@@ -3584,11 +3584,11 @@
       <c r="O5" s="14"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="45"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
@@ -3601,11 +3601,11 @@
       <c r="O6" s="14"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="45"/>
-      <c r="B7" s="45"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -3618,11 +3618,11 @@
       <c r="O7" s="14"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="45"/>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -3635,11 +3635,11 @@
       <c r="O8" s="14"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="46"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
+      <c r="A9" s="37"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="37"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -5074,9 +5074,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A31FFDAE-1104-4CD3-91B9-BF5E1B8C8EDE}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17:H19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="103" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5280,13 +5280,13 @@
         <v>16</v>
       </c>
       <c r="F17" s="3">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="G17" s="3">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="H17" s="3">
-        <v>9</v>
+        <v>9.5</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3" t="s">
@@ -5368,7 +5368,9 @@
         <v>15</v>
       </c>
       <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -5389,7 +5391,9 @@
       <c r="E21" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="3"/>
+      <c r="F21" s="3">
+        <v>2</v>
+      </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -5413,7 +5417,9 @@
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
+      <c r="H22" s="3">
+        <v>0.5</v>
+      </c>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
     </row>
@@ -5435,7 +5441,9 @@
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
+      <c r="H23" s="3">
+        <v>6</v>
+      </c>
       <c r="I23" s="3"/>
       <c r="J23" s="3"/>
     </row>
@@ -5456,7 +5464,9 @@
         <v>15</v>
       </c>
       <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="G24" s="3">
+        <v>3</v>
+      </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
@@ -5479,7 +5489,9 @@
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
+      <c r="H25" s="3">
+        <v>3</v>
+      </c>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
@@ -5553,15 +5565,15 @@
       </c>
       <c r="F31" s="5">
         <f>SUM(F17:F30)</f>
-        <v>10</v>
+        <v>12.5</v>
       </c>
       <c r="G31" s="5">
         <f t="shared" ref="G31:I31" si="0">SUM(G17:G30)</f>
-        <v>10</v>
+        <v>14.5</v>
       </c>
       <c r="H31" s="5">
         <f t="shared" si="0"/>
-        <v>10.5</v>
+        <v>20.5</v>
       </c>
       <c r="I31" s="5">
         <f t="shared" si="0"/>
@@ -5603,150 +5615,144 @@
       <c r="A36" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="39"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="39"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="39"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="39"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -5756,6 +5762,12 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -6150,144 +6162,150 @@
       <c r="A36" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="39"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="39"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="39"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="39"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -6297,12 +6315,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -6697,144 +6709,150 @@
       <c r="A36" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="39"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="39"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="39"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="39"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -6844,12 +6862,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -7244,144 +7256,150 @@
       <c r="A36" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="39"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="39"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="39"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="39"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -7391,12 +7409,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -7791,144 +7803,150 @@
       <c r="A36" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="39"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="39"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="39"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="39"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -7938,12 +7956,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -8338,144 +8350,150 @@
       <c r="A36" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B36" s="36"/>
-      <c r="C36" s="36"/>
-      <c r="D36" s="36"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
-      <c r="G36" s="36"/>
-      <c r="H36" s="36"/>
-      <c r="I36" s="36"/>
-      <c r="J36" s="37"/>
+      <c r="B36" s="38"/>
+      <c r="C36" s="38"/>
+      <c r="D36" s="38"/>
+      <c r="E36" s="38"/>
+      <c r="F36" s="38"/>
+      <c r="G36" s="38"/>
+      <c r="H36" s="38"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="B37" s="36"/>
-      <c r="C37" s="36"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="36"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="36"/>
-      <c r="H37" s="36"/>
-      <c r="I37" s="36"/>
-      <c r="J37" s="37"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="38"/>
+      <c r="D37" s="38"/>
+      <c r="E37" s="38"/>
+      <c r="F37" s="38"/>
+      <c r="G37" s="38"/>
+      <c r="H37" s="38"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="39"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="D38" s="36"/>
-      <c r="E38" s="36"/>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36"/>
-      <c r="H38" s="36"/>
-      <c r="I38" s="36"/>
-      <c r="J38" s="37"/>
+      <c r="B38" s="38"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="38"/>
+      <c r="I38" s="38"/>
+      <c r="J38" s="39"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B39" s="36"/>
-      <c r="C39" s="36"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="36"/>
-      <c r="F39" s="36"/>
-      <c r="G39" s="36"/>
-      <c r="H39" s="36"/>
-      <c r="I39" s="36"/>
-      <c r="J39" s="37"/>
+      <c r="B39" s="38"/>
+      <c r="C39" s="38"/>
+      <c r="D39" s="38"/>
+      <c r="E39" s="38"/>
+      <c r="F39" s="38"/>
+      <c r="G39" s="38"/>
+      <c r="H39" s="38"/>
+      <c r="I39" s="38"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="36"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="36"/>
-      <c r="H40" s="36"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="37"/>
+      <c r="B40" s="38"/>
+      <c r="C40" s="38"/>
+      <c r="D40" s="38"/>
+      <c r="E40" s="38"/>
+      <c r="F40" s="38"/>
+      <c r="G40" s="38"/>
+      <c r="H40" s="38"/>
+      <c r="I40" s="38"/>
+      <c r="J40" s="39"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="36"/>
-      <c r="F41" s="36"/>
-      <c r="G41" s="36"/>
-      <c r="H41" s="36"/>
-      <c r="I41" s="36"/>
-      <c r="J41" s="37"/>
+      <c r="B41" s="38"/>
+      <c r="C41" s="38"/>
+      <c r="D41" s="38"/>
+      <c r="E41" s="38"/>
+      <c r="F41" s="38"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="38"/>
+      <c r="I41" s="38"/>
+      <c r="J41" s="39"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="36"/>
-      <c r="D42" s="36"/>
-      <c r="E42" s="36"/>
-      <c r="F42" s="36"/>
-      <c r="G42" s="36"/>
-      <c r="H42" s="36"/>
-      <c r="I42" s="36"/>
-      <c r="J42" s="37"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="38"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="38"/>
+      <c r="G42" s="38"/>
+      <c r="H42" s="38"/>
+      <c r="I42" s="38"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B43" s="36"/>
-      <c r="C43" s="36"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="36"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="36"/>
-      <c r="H43" s="36"/>
-      <c r="I43" s="36"/>
-      <c r="J43" s="37"/>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="36"/>
-      <c r="C44" s="36"/>
-      <c r="D44" s="36"/>
-      <c r="E44" s="36"/>
-      <c r="F44" s="36"/>
-      <c r="G44" s="36"/>
-      <c r="H44" s="36"/>
-      <c r="I44" s="36"/>
-      <c r="J44" s="37"/>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="39"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="38"/>
-      <c r="C45" s="38"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="38"/>
-      <c r="F45" s="38"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
-      <c r="J45" s="39"/>
+      <c r="B45" s="45"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="45"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="45"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -8485,12 +8503,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -8500,6 +8512,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009EB83581AE75E3448E2425BE2C4A9358" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="3613ffd620ebef032c0b03220f523539">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87f001ec-f7b3-49be-8676-481a173a404e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="972cec87c5ab16132ba820573bf22a25" ns2:_="">
     <xsd:import namespace="87f001ec-f7b3-49be-8676-481a173a404e"/>
@@ -8631,12 +8649,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8647,6 +8659,22 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{959E2576-8ACA-4472-AE2B-4AF07B9AFF6B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="87f001ec-f7b3-49be-8676-481a173a404e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5025CB3-4618-43BF-8CBB-8A6ABF966F86}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8664,22 +8692,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{959E2576-8ACA-4472-AE2B-4AF07B9AFF6B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="87f001ec-f7b3-49be-8676-481a173a404e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05AA98B7-DD2A-4000-A348-80CCBB56207C}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
SCRUM planning mistake fixed
</commit_message>
<xml_diff>
--- a/Docs/Scrum planning en rapport template.xlsx
+++ b/Docs/Scrum planning en rapport template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecr\Documents\AP\2eJ-semester2\AI Project\AI-Project\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B55863-AE16-4108-8C1F-627C45D40019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE03422A-7895-4DE6-8D1B-088C8AA5F088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{E07F6153-1B8C-43A7-97BD-457FD435295E}"/>
   </bookViews>
@@ -1284,6 +1284,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1293,8 +1295,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="D8">
         <f>'Sprint 0'!F31+'Sprint 1'!F31+'Sprint 2'!F31+'Sprint 3'!F31+'Sprint 4'!F31+'Sprint 5'!F31+'Sprint 6'!F31+'Sprint 7'!F31</f>
-        <v>12.5</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="D10">
         <f>'Sprint 0'!H31+'Sprint 1'!H31+'Sprint 2'!H31+'Sprint 3'!H31+'Sprint 4'!H31+'Sprint 5'!H31+'Sprint 6'!H31+'Sprint 7'!H31</f>
-        <v>20.5</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -2461,30 +2461,30 @@
       <c r="B9" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
     </row>
     <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
@@ -2502,12 +2502,12 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -2753,17 +2753,17 @@
       <c r="A35" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="44"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="46"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
@@ -2895,24 +2895,18 @@
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="46"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -2922,6 +2916,12 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -3008,30 +3008,30 @@
       <c r="B9" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
     </row>
     <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
@@ -3049,12 +3049,12 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -3300,17 +3300,17 @@
       <c r="A35" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="44"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="46"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
@@ -3442,24 +3442,18 @@
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="46"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -3469,6 +3463,12 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -5076,7 +5076,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="103" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+      <selection pane="bottomLeft" activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5169,32 +5169,32 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:13" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
     </row>
     <row r="14" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
@@ -5212,12 +5212,12 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
       <c r="L15" s="2" t="s">
         <v>7</v>
       </c>
@@ -5487,11 +5487,11 @@
       <c r="E25" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="3"/>
+      <c r="F25" s="3">
+        <v>3</v>
+      </c>
       <c r="G25" s="3"/>
-      <c r="H25" s="3">
-        <v>3</v>
-      </c>
+      <c r="H25" s="3"/>
       <c r="I25" s="3"/>
       <c r="J25" s="3"/>
     </row>
@@ -5565,7 +5565,7 @@
       </c>
       <c r="F31" s="5">
         <f>SUM(F17:F30)</f>
-        <v>12.5</v>
+        <v>15.5</v>
       </c>
       <c r="G31" s="5">
         <f t="shared" ref="G31:I31" si="0">SUM(G17:G30)</f>
@@ -5573,7 +5573,7 @@
       </c>
       <c r="H31" s="5">
         <f t="shared" si="0"/>
-        <v>20.5</v>
+        <v>17.5</v>
       </c>
       <c r="I31" s="5">
         <f t="shared" si="0"/>
@@ -5599,17 +5599,17 @@
       <c r="A35" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="44"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="46"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
@@ -5741,18 +5741,24 @@
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="46"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -5762,12 +5768,6 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -5854,30 +5854,30 @@
       <c r="B9" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
     </row>
     <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
@@ -5895,12 +5895,12 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -6146,17 +6146,17 @@
       <c r="A35" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="44"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="46"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
@@ -6288,24 +6288,18 @@
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="46"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -6315,6 +6309,12 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -6401,30 +6401,30 @@
       <c r="B9" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
     </row>
     <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
@@ -6442,12 +6442,12 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -6693,17 +6693,17 @@
       <c r="A35" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="44"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="46"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
@@ -6835,24 +6835,18 @@
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="46"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -6862,6 +6856,12 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -6948,30 +6948,30 @@
       <c r="B9" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
     </row>
     <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
@@ -6989,12 +6989,12 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -7240,17 +7240,17 @@
       <c r="A35" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="44"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="46"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
@@ -7382,24 +7382,18 @@
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="46"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -7409,6 +7403,12 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -7495,30 +7495,30 @@
       <c r="B9" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
     </row>
     <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
@@ -7536,12 +7536,12 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -7787,17 +7787,17 @@
       <c r="A35" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="44"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="46"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
@@ -7929,24 +7929,18 @@
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="46"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -7956,6 +7950,12 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -8042,30 +8042,30 @@
       <c r="B9" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="42"/>
     </row>
     <row r="12" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
+      <c r="A12" s="43"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
     </row>
     <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
@@ -8083,12 +8083,12 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
-      <c r="F15" s="42" t="s">
+      <c r="F15" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="44"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -8334,17 +8334,17 @@
       <c r="A35" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="B35" s="43" t="s">
+      <c r="B35" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="44"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="45"/>
+      <c r="G35" s="45"/>
+      <c r="H35" s="45"/>
+      <c r="I35" s="45"/>
+      <c r="J35" s="46"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="12" t="s">
@@ -8476,24 +8476,18 @@
       <c r="A45" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="45"/>
-      <c r="C45" s="45"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="45"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="45"/>
-      <c r="I45" s="45"/>
-      <c r="J45" s="46"/>
+      <c r="B45" s="40"/>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="40"/>
+      <c r="G45" s="40"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B36:J36"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A12:J12"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="B35:J35"/>
     <mergeCell ref="B43:J43"/>
     <mergeCell ref="B44:J44"/>
     <mergeCell ref="B45:J45"/>
@@ -8503,6 +8497,12 @@
     <mergeCell ref="B40:J40"/>
     <mergeCell ref="B41:J41"/>
     <mergeCell ref="B42:J42"/>
+    <mergeCell ref="B36:J36"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="B35:J35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -8512,12 +8512,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101009EB83581AE75E3448E2425BE2C4A9358" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="3613ffd620ebef032c0b03220f523539">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87f001ec-f7b3-49be-8676-481a173a404e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="972cec87c5ab16132ba820573bf22a25" ns2:_="">
     <xsd:import namespace="87f001ec-f7b3-49be-8676-481a173a404e"/>
@@ -8649,6 +8643,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -8659,22 +8659,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{959E2576-8ACA-4472-AE2B-4AF07B9AFF6B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="87f001ec-f7b3-49be-8676-481a173a404e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E5025CB3-4618-43BF-8CBB-8A6ABF966F86}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8692,6 +8676,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{959E2576-8ACA-4472-AE2B-4AF07B9AFF6B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="87f001ec-f7b3-49be-8676-481a173a404e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{05AA98B7-DD2A-4000-A348-80CCBB56207C}">
   <ds:schemaRefs>

</xml_diff>